<commit_message>
08-02, se kalo dromo no9
</commit_message>
<xml_diff>
--- a/django-final.xlsx
+++ b/django-final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALEXIS\OneDrive\PYTHON-LESSONS\DJANGO-ALL\instruments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d806637bdf860dec/PYTHON-LESSONS/DJANGO-ALL/instruments_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08230B76-CFB9-44EB-A19D-2CB7270D7DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{08230B76-CFB9-44EB-A19D-2CB7270D7DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B32423-14FC-46AE-BF78-A3AFF3892E62}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{FB5333B4-F737-4A71-BEF7-FEEE3BBE2E90}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FB5333B4-F737-4A71-BEF7-FEEE3BBE2E90}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <r>
       <t>·</t>
@@ -812,12 +812,60 @@
   <si>
     <t>εφτιαξε αυτοματα static dir και στο main root, με καποια (πολλα) επιπλέον.</t>
   </si>
+  <si>
+    <t>GITHUB</t>
+  </si>
+  <si>
+    <t>φτιαχνω νέο reposatory</t>
+  </si>
+  <si>
+    <t>δινω το ιδιο ονομα</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>gitignore</t>
+  </si>
+  <si>
+    <t>*.log
+*.pot
+*.pyc
+__pycache__/
+local_settings.py
+db.sqlite3
+db.sqlite3-journal
+/media
+venv
+/static</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>git commit -m "comments"</t>
+  </si>
+  <si>
+    <t>από github https or SSH και με αντιγραφη εντολων, παλι παω στο terminal</t>
+  </si>
+  <si>
+    <t>git remote add origin ….................</t>
+  </si>
+  <si>
+    <t>git push -u origin master</t>
+  </si>
+  <si>
+    <t>https://gist.github.com/bradtraversy/cfa565b879ff1458dba08f423cb01d71</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -888,6 +936,15 @@
       <family val="1"/>
       <charset val="161"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -912,10 +969,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -947,9 +1005,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Υπερ-σύνδεση" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1346,7 +1406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1354,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEAB3A0-2607-4CD9-B7FE-F6E3A16F6CBA}">
-  <dimension ref="B2:C76"/>
+  <dimension ref="B2:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,7 +1783,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="2:2" ht="150" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" ht="165" x14ac:dyDescent="0.25">
       <c r="B73" s="6" t="s">
         <v>69</v>
       </c>
@@ -1733,7 +1793,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" spans="2:2" ht="240" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" ht="255" x14ac:dyDescent="0.25">
       <c r="B75" s="6" t="s">
         <v>70</v>
       </c>
@@ -1743,10 +1803,76 @@
         <v>72</v>
       </c>
     </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="B85" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B92" r:id="rId1" xr:uid="{1721EA83-6E31-4F93-A285-DB990D7D3B30}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
14-02, se kalo dromo no11
</commit_message>
<xml_diff>
--- a/django-final.xlsx
+++ b/django-final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d806637bdf860dec/PYTHON-LESSONS/DJANGO-ALL/instruments_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{08230B76-CFB9-44EB-A19D-2CB7270D7DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93B32423-14FC-46AE-BF78-A3AFF3892E62}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{08230B76-CFB9-44EB-A19D-2CB7270D7DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{129C51F3-1F57-4F96-A07A-0EB5B67EBD36}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{FB5333B4-F737-4A71-BEF7-FEEE3BBE2E90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB5333B4-F737-4A71-BEF7-FEEE3BBE2E90}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -810,9 +810,6 @@
     </r>
   </si>
   <si>
-    <t>εφτιαξε αυτοματα static dir και στο main root, με καποια (πολλα) επιπλέον.</t>
-  </si>
-  <si>
     <t>GITHUB</t>
   </si>
   <si>
@@ -859,6 +856,9 @@
   </si>
   <si>
     <t>https://gist.github.com/bradtraversy/cfa565b879ff1458dba08f423cb01d71</t>
+  </si>
+  <si>
+    <t>εφτιαξε αυτοματα static dir και στο main root, με καποια (πολλα) επιπλέον. Μετα από αυτην κίνηση, ότι βάζω στο instruments/static με collectstatic αντιγράφεται στο main root static</t>
   </si>
 </sst>
 </file>
@@ -1115,6 +1115,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1416,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEAB3A0-2607-4CD9-B7FE-F6E3A16F6CBA}">
   <dimension ref="B2:C92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1653,9 +1657,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" ht="60" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="150" x14ac:dyDescent="0.25">
@@ -1805,65 +1809,65 @@
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="150" x14ac:dyDescent="0.25">
       <c r="B85" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B86" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>